<commit_message>
structure codes withs much interfaces
</commit_message>
<xml_diff>
--- a/KylinGame/release/configfile/dataConfig/item/itemSheetData.xlsx
+++ b/KylinGame/release/configfile/dataConfig/item/itemSheetData.xlsx
@@ -899,9 +899,6 @@
     <t>usageDesc</t>
   </si>
   <si>
-    <t>resourceId</t>
-  </si>
-  <si>
     <t>canAskFor</t>
   </si>
   <si>
@@ -2471,6 +2468,10 @@
   </si>
   <si>
     <t>ItemName_133148</t>
+  </si>
+  <si>
+    <t>resId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3010,10 +3011,10 @@
   <dimension ref="A1:Z246"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3124,7 +3125,7 @@
         <v>24</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15.95" customHeight="1">
@@ -3195,16 +3196,16 @@
         <v>46</v>
       </c>
       <c r="W2" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="X2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="Z2" s="6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5">
@@ -3212,10 +3213,10 @@
         <v>131050</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="D3" s="5">
         <v>3</v>
@@ -3276,10 +3277,10 @@
         <v>131051</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
@@ -3340,10 +3341,10 @@
         <v>131052</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
@@ -3404,10 +3405,10 @@
         <v>131053</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
@@ -3468,10 +3469,10 @@
         <v>131054</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
@@ -3532,10 +3533,10 @@
         <v>131055</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
@@ -3596,10 +3597,10 @@
         <v>131056</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="D9" s="5">
         <v>1</v>
@@ -3660,10 +3661,10 @@
         <v>131057</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>65</v>
       </c>
       <c r="D10" s="5">
         <v>1</v>
@@ -3724,10 +3725,10 @@
         <v>131060</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="D11" s="5">
         <v>3</v>
@@ -3792,10 +3793,10 @@
         <v>131061</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="D12" s="5">
         <v>1</v>
@@ -3811,7 +3812,7 @@
         <v>3</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="J12" s="5">
         <v>2</v>
@@ -3862,10 +3863,10 @@
         <v>131063</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="D13" s="5">
         <v>1</v>
@@ -3881,7 +3882,7 @@
         <v>3</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="J13" s="5">
         <v>2</v>
@@ -3932,10 +3933,10 @@
         <v>131064</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="D14" s="5">
         <v>1</v>
@@ -3998,10 +3999,10 @@
         <v>131065</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
@@ -4064,10 +4065,10 @@
         <v>131066</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="D16" s="5">
         <v>1</v>
@@ -4130,10 +4131,10 @@
         <v>131067</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="D17" s="5">
         <v>1</v>
@@ -4200,10 +4201,10 @@
         <v>131068</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="D18" s="5">
         <v>1</v>
@@ -4270,10 +4271,10 @@
         <v>131069</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="D19" s="5">
         <v>1</v>
@@ -4340,10 +4341,10 @@
         <v>131070</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="D20" s="5">
         <v>1</v>
@@ -4410,10 +4411,10 @@
         <v>131071</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>87</v>
       </c>
       <c r="D21" s="5">
         <v>1</v>
@@ -4474,10 +4475,10 @@
         <v>131072</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="D22" s="5">
         <v>1</v>
@@ -4493,7 +4494,7 @@
         <v>1</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5">
@@ -4540,10 +4541,10 @@
         <v>131073</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="D23" s="5">
         <v>1</v>
@@ -4604,10 +4605,10 @@
         <v>131074</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="D24" s="5">
         <v>1</v>
@@ -4668,10 +4669,10 @@
         <v>131075</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="D25" s="5">
         <v>1</v>
@@ -4732,10 +4733,10 @@
         <v>131076</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="D26" s="5">
         <v>1</v>
@@ -4796,10 +4797,10 @@
         <v>131077</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="D27" s="5">
         <v>1</v>
@@ -4815,7 +4816,7 @@
         <v>1</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5">
@@ -4862,10 +4863,10 @@
         <v>131078</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="D28" s="5">
         <v>1</v>
@@ -4881,7 +4882,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5">
@@ -4928,10 +4929,10 @@
         <v>131079</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="D29" s="5">
         <v>1</v>
@@ -4947,7 +4948,7 @@
         <v>1</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5">
@@ -4994,10 +4995,10 @@
         <v>131080</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>109</v>
       </c>
       <c r="D30" s="5">
         <v>1</v>
@@ -5013,7 +5014,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5">
@@ -5060,10 +5061,10 @@
         <v>131081</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="D31" s="5">
         <v>1</v>
@@ -5079,7 +5080,7 @@
         <v>1</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5">
@@ -5126,10 +5127,10 @@
         <v>131082</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>115</v>
       </c>
       <c r="D32" s="5">
         <v>1</v>
@@ -5145,7 +5146,7 @@
         <v>1</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5">
@@ -5192,10 +5193,10 @@
         <v>131083</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="D33" s="5">
         <v>1</v>
@@ -5211,7 +5212,7 @@
         <v>1</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5">
@@ -5258,10 +5259,10 @@
         <v>131086</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="D34" s="5">
         <v>1</v>
@@ -5277,7 +5278,7 @@
         <v>1</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5">
@@ -5324,10 +5325,10 @@
         <v>131087</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="D35" s="5">
         <v>1</v>
@@ -5343,7 +5344,7 @@
         <v>1</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="5">
@@ -5390,10 +5391,10 @@
         <v>131088</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>127</v>
       </c>
       <c r="D36" s="9">
         <v>1</v>
@@ -5409,7 +5410,7 @@
         <v>1</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="J36" s="9"/>
       <c r="K36" s="5">
@@ -5458,10 +5459,10 @@
         <v>131091</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="D37" s="9">
         <v>1</v>
@@ -5477,7 +5478,7 @@
         <v>1</v>
       </c>
       <c r="I37" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J37" s="9"/>
       <c r="K37" s="5">
@@ -5526,10 +5527,10 @@
         <v>131092</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>131</v>
       </c>
       <c r="D38" s="9">
         <v>1</v>
@@ -5545,7 +5546,7 @@
         <v>1</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J38" s="9">
         <v>2</v>
@@ -5598,10 +5599,10 @@
         <v>131095</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="D39" s="9">
         <v>1</v>
@@ -5617,7 +5618,7 @@
         <v>1</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J39" s="9">
         <v>2</v>
@@ -5670,10 +5671,10 @@
         <v>131104</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="D40" s="9">
         <v>1</v>
@@ -5689,7 +5690,7 @@
         <v>1</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J40" s="9"/>
       <c r="K40" s="5">
@@ -5738,10 +5739,10 @@
         <v>131107</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="D41" s="9">
         <v>1</v>
@@ -5757,7 +5758,7 @@
         <v>1</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J41" s="9"/>
       <c r="K41" s="5">
@@ -5806,10 +5807,10 @@
         <v>131108</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D42" s="5">
         <v>1</v>
@@ -5870,10 +5871,10 @@
         <v>131109</v>
       </c>
       <c r="B43" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="D43" s="5">
         <v>1</v>
@@ -5934,10 +5935,10 @@
         <v>131110</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="D44" s="5">
         <v>1</v>
@@ -5998,10 +5999,10 @@
         <v>131111</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>147</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>148</v>
       </c>
       <c r="D45" s="5">
         <v>1</v>
@@ -6062,10 +6063,10 @@
         <v>131112</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="D46" s="5">
         <v>1</v>
@@ -6126,10 +6127,10 @@
         <v>131113</v>
       </c>
       <c r="B47" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>151</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>152</v>
       </c>
       <c r="D47" s="5">
         <v>1</v>
@@ -6190,10 +6191,10 @@
         <v>131114</v>
       </c>
       <c r="B48" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="D48" s="5">
         <v>1</v>
@@ -6254,10 +6255,10 @@
         <v>131122</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D49" s="5">
         <v>1</v>
@@ -6318,10 +6319,10 @@
         <v>131115</v>
       </c>
       <c r="B50" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C50" s="10" t="s">
         <v>156</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>157</v>
       </c>
       <c r="D50" s="5">
         <v>1</v>
@@ -6384,10 +6385,10 @@
         <v>131116</v>
       </c>
       <c r="B51" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" s="10" t="s">
         <v>158</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>159</v>
       </c>
       <c r="D51" s="5">
         <v>1</v>
@@ -6450,10 +6451,10 @@
         <v>131117</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D52" s="5">
         <v>1</v>
@@ -6516,10 +6517,10 @@
         <v>131123</v>
       </c>
       <c r="B53" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="C53" s="10" t="s">
         <v>489</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>490</v>
       </c>
       <c r="D53" s="5">
         <v>1</v>
@@ -6578,10 +6579,10 @@
         <v>131118</v>
       </c>
       <c r="B54" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>162</v>
       </c>
       <c r="D54" s="8">
         <v>1</v>
@@ -6642,10 +6643,10 @@
         <v>131119</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D55" s="5">
         <v>1</v>
@@ -6706,10 +6707,10 @@
         <v>131120</v>
       </c>
       <c r="B56" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="D56" s="5">
         <v>1</v>
@@ -6770,10 +6771,10 @@
         <v>131121</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D57" s="5">
         <v>1</v>
@@ -6834,10 +6835,10 @@
         <v>131124</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D58" s="11">
         <v>1</v>
@@ -6853,7 +6854,7 @@
         <v>1</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J58" s="11">
         <v>2</v>
@@ -6902,10 +6903,10 @@
         <v>131125</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D59" s="11">
         <v>1</v>
@@ -6921,7 +6922,7 @@
         <v>1</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="J59" s="11">
         <v>2</v>
@@ -6970,10 +6971,10 @@
         <v>131126</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D60" s="5">
         <v>1</v>
@@ -6989,7 +6990,7 @@
         <v>15</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J60" s="5">
         <v>2</v>
@@ -7038,10 +7039,10 @@
         <v>131127</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D61" s="5">
         <v>1</v>
@@ -7057,7 +7058,7 @@
         <v>15</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="J61" s="5">
         <v>2</v>
@@ -7106,10 +7107,10 @@
         <v>131128</v>
       </c>
       <c r="B62" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="C62" s="13" t="s">
         <v>501</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>502</v>
       </c>
       <c r="D62" s="5">
         <v>1</v>
@@ -7170,10 +7171,10 @@
         <v>132001</v>
       </c>
       <c r="B63" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C63" s="13" t="s">
         <v>167</v>
-      </c>
-      <c r="C63" s="13" t="s">
-        <v>168</v>
       </c>
       <c r="D63" s="5">
         <v>2</v>
@@ -7236,10 +7237,10 @@
         <v>132002</v>
       </c>
       <c r="B64" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C64" s="13" t="s">
         <v>169</v>
-      </c>
-      <c r="C64" s="13" t="s">
-        <v>170</v>
       </c>
       <c r="D64" s="5">
         <v>2</v>
@@ -7302,10 +7303,10 @@
         <v>132003</v>
       </c>
       <c r="B65" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C65" s="13" t="s">
         <v>171</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>172</v>
       </c>
       <c r="D65" s="5">
         <v>2</v>
@@ -7368,10 +7369,10 @@
         <v>132004</v>
       </c>
       <c r="B66" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="C66" s="13" t="s">
         <v>503</v>
-      </c>
-      <c r="C66" s="13" t="s">
-        <v>504</v>
       </c>
       <c r="D66" s="5">
         <v>2</v>
@@ -7432,10 +7433,10 @@
         <v>132005</v>
       </c>
       <c r="B67" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="C67" s="13" t="s">
         <v>505</v>
-      </c>
-      <c r="C67" s="13" t="s">
-        <v>506</v>
       </c>
       <c r="D67" s="5">
         <v>2</v>
@@ -7494,10 +7495,10 @@
         <v>133001</v>
       </c>
       <c r="B68" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="D68" s="5">
         <v>3</v>
@@ -7560,10 +7561,10 @@
         <v>133002</v>
       </c>
       <c r="B69" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C69" s="5" t="s">
         <v>175</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>176</v>
       </c>
       <c r="D69" s="5">
         <v>3</v>
@@ -7626,10 +7627,10 @@
         <v>133003</v>
       </c>
       <c r="B70" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>178</v>
       </c>
       <c r="D70" s="5">
         <v>3</v>
@@ -7692,10 +7693,10 @@
         <v>133004</v>
       </c>
       <c r="B71" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>180</v>
       </c>
       <c r="D71" s="5">
         <v>3</v>
@@ -7758,10 +7759,10 @@
         <v>133005</v>
       </c>
       <c r="B72" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C72" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>182</v>
       </c>
       <c r="D72" s="5">
         <v>3</v>
@@ -7824,10 +7825,10 @@
         <v>133006</v>
       </c>
       <c r="B73" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C73" s="5" t="s">
         <v>183</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>184</v>
       </c>
       <c r="D73" s="5">
         <v>3</v>
@@ -7890,10 +7891,10 @@
         <v>133007</v>
       </c>
       <c r="B74" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>185</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>186</v>
       </c>
       <c r="D74" s="5">
         <v>3</v>
@@ -7956,10 +7957,10 @@
         <v>133008</v>
       </c>
       <c r="B75" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C75" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>188</v>
       </c>
       <c r="D75" s="5">
         <v>3</v>
@@ -8022,10 +8023,10 @@
         <v>133009</v>
       </c>
       <c r="B76" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>190</v>
       </c>
       <c r="D76" s="5">
         <v>3</v>
@@ -8088,10 +8089,10 @@
         <v>133010</v>
       </c>
       <c r="B77" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C77" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="D77" s="5">
         <v>3</v>
@@ -8154,10 +8155,10 @@
         <v>133011</v>
       </c>
       <c r="B78" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C78" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="D78" s="5">
         <v>3</v>
@@ -8220,10 +8221,10 @@
         <v>133012</v>
       </c>
       <c r="B79" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C79" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>196</v>
       </c>
       <c r="D79" s="5">
         <v>3</v>
@@ -8286,10 +8287,10 @@
         <v>133013</v>
       </c>
       <c r="B80" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C80" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="D80" s="5">
         <v>3</v>
@@ -8352,10 +8353,10 @@
         <v>133014</v>
       </c>
       <c r="B81" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C81" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="D81" s="5">
         <v>3</v>
@@ -8418,10 +8419,10 @@
         <v>133015</v>
       </c>
       <c r="B82" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C82" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>202</v>
       </c>
       <c r="D82" s="5">
         <v>3</v>
@@ -8484,10 +8485,10 @@
         <v>133016</v>
       </c>
       <c r="B83" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C83" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>204</v>
       </c>
       <c r="D83" s="5">
         <v>3</v>
@@ -8550,10 +8551,10 @@
         <v>133017</v>
       </c>
       <c r="B84" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C84" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="D84" s="5">
         <v>3</v>
@@ -8616,10 +8617,10 @@
         <v>133018</v>
       </c>
       <c r="B85" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C85" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>208</v>
       </c>
       <c r="D85" s="5">
         <v>3</v>
@@ -8682,10 +8683,10 @@
         <v>133019</v>
       </c>
       <c r="B86" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C86" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>210</v>
       </c>
       <c r="D86" s="5">
         <v>3</v>
@@ -8748,10 +8749,10 @@
         <v>133020</v>
       </c>
       <c r="B87" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C87" s="5" t="s">
         <v>211</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>212</v>
       </c>
       <c r="D87" s="5">
         <v>3</v>
@@ -8814,10 +8815,10 @@
         <v>133021</v>
       </c>
       <c r="B88" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C88" s="5" t="s">
         <v>213</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>214</v>
       </c>
       <c r="D88" s="5">
         <v>3</v>
@@ -8880,10 +8881,10 @@
         <v>133022</v>
       </c>
       <c r="B89" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C89" s="5" t="s">
         <v>215</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>216</v>
       </c>
       <c r="D89" s="5">
         <v>3</v>
@@ -8946,10 +8947,10 @@
         <v>133023</v>
       </c>
       <c r="B90" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C90" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>218</v>
       </c>
       <c r="D90" s="5">
         <v>3</v>
@@ -9012,10 +9013,10 @@
         <v>133024</v>
       </c>
       <c r="B91" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C91" s="5" t="s">
         <v>219</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>220</v>
       </c>
       <c r="D91" s="5">
         <v>3</v>
@@ -9078,10 +9079,10 @@
         <v>133025</v>
       </c>
       <c r="B92" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C92" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>222</v>
       </c>
       <c r="D92" s="5">
         <v>3</v>
@@ -9144,10 +9145,10 @@
         <v>133026</v>
       </c>
       <c r="B93" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C93" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="D93" s="5">
         <v>3</v>
@@ -9210,10 +9211,10 @@
         <v>133027</v>
       </c>
       <c r="B94" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C94" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>226</v>
       </c>
       <c r="D94" s="5">
         <v>3</v>
@@ -9276,10 +9277,10 @@
         <v>133028</v>
       </c>
       <c r="B95" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C95" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>228</v>
       </c>
       <c r="D95" s="5">
         <v>3</v>
@@ -9342,10 +9343,10 @@
         <v>133029</v>
       </c>
       <c r="B96" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C96" s="5" t="s">
         <v>229</v>
-      </c>
-      <c r="C96" s="5" t="s">
-        <v>230</v>
       </c>
       <c r="D96" s="5">
         <v>3</v>
@@ -9408,10 +9409,10 @@
         <v>133030</v>
       </c>
       <c r="B97" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C97" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>232</v>
       </c>
       <c r="D97" s="5">
         <v>3</v>
@@ -9474,10 +9475,10 @@
         <v>133031</v>
       </c>
       <c r="B98" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C98" s="5" t="s">
         <v>233</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>234</v>
       </c>
       <c r="D98" s="5">
         <v>3</v>
@@ -9540,10 +9541,10 @@
         <v>133032</v>
       </c>
       <c r="B99" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C99" s="5" t="s">
         <v>235</v>
-      </c>
-      <c r="C99" s="5" t="s">
-        <v>236</v>
       </c>
       <c r="D99" s="5">
         <v>3</v>
@@ -9610,10 +9611,10 @@
         <v>133033</v>
       </c>
       <c r="B100" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C100" s="5" t="s">
         <v>237</v>
-      </c>
-      <c r="C100" s="5" t="s">
-        <v>238</v>
       </c>
       <c r="D100" s="5">
         <v>3</v>
@@ -9676,10 +9677,10 @@
         <v>133034</v>
       </c>
       <c r="B101" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C101" s="5" t="s">
         <v>239</v>
-      </c>
-      <c r="C101" s="5" t="s">
-        <v>240</v>
       </c>
       <c r="D101" s="5">
         <v>3</v>
@@ -9742,10 +9743,10 @@
         <v>133035</v>
       </c>
       <c r="B102" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C102" s="5" t="s">
         <v>241</v>
-      </c>
-      <c r="C102" s="5" t="s">
-        <v>242</v>
       </c>
       <c r="D102" s="5">
         <v>3</v>
@@ -9808,10 +9809,10 @@
         <v>133036</v>
       </c>
       <c r="B103" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C103" s="5" t="s">
         <v>243</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>244</v>
       </c>
       <c r="D103" s="5">
         <v>3</v>
@@ -9874,10 +9875,10 @@
         <v>133037</v>
       </c>
       <c r="B104" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C104" s="5" t="s">
         <v>245</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>246</v>
       </c>
       <c r="D104" s="5">
         <v>3</v>
@@ -9940,10 +9941,10 @@
         <v>133038</v>
       </c>
       <c r="B105" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C105" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="C105" s="5" t="s">
-        <v>248</v>
       </c>
       <c r="D105" s="5">
         <v>3</v>
@@ -10006,10 +10007,10 @@
         <v>133039</v>
       </c>
       <c r="B106" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C106" s="5" t="s">
         <v>249</v>
-      </c>
-      <c r="C106" s="5" t="s">
-        <v>250</v>
       </c>
       <c r="D106" s="5">
         <v>3</v>
@@ -10072,10 +10073,10 @@
         <v>133040</v>
       </c>
       <c r="B107" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C107" s="5" t="s">
         <v>251</v>
-      </c>
-      <c r="C107" s="5" t="s">
-        <v>252</v>
       </c>
       <c r="D107" s="5">
         <v>3</v>
@@ -10134,10 +10135,10 @@
         <v>133041</v>
       </c>
       <c r="B108" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C108" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>254</v>
       </c>
       <c r="D108" s="5">
         <v>3</v>
@@ -10200,10 +10201,10 @@
         <v>133042</v>
       </c>
       <c r="B109" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C109" s="5" t="s">
         <v>255</v>
-      </c>
-      <c r="C109" s="5" t="s">
-        <v>256</v>
       </c>
       <c r="D109" s="5">
         <v>3</v>
@@ -10266,10 +10267,10 @@
         <v>133043</v>
       </c>
       <c r="B110" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C110" s="5" t="s">
         <v>257</v>
-      </c>
-      <c r="C110" s="5" t="s">
-        <v>258</v>
       </c>
       <c r="D110" s="5">
         <v>3</v>
@@ -10332,10 +10333,10 @@
         <v>133044</v>
       </c>
       <c r="B111" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C111" s="5" t="s">
         <v>259</v>
-      </c>
-      <c r="C111" s="5" t="s">
-        <v>260</v>
       </c>
       <c r="D111" s="5">
         <v>3</v>
@@ -10398,10 +10399,10 @@
         <v>133045</v>
       </c>
       <c r="B112" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C112" s="5" t="s">
         <v>261</v>
-      </c>
-      <c r="C112" s="5" t="s">
-        <v>262</v>
       </c>
       <c r="D112" s="5">
         <v>3</v>
@@ -10464,10 +10465,10 @@
         <v>133046</v>
       </c>
       <c r="B113" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C113" s="5" t="s">
         <v>263</v>
-      </c>
-      <c r="C113" s="5" t="s">
-        <v>264</v>
       </c>
       <c r="D113" s="5">
         <v>3</v>
@@ -10534,10 +10535,10 @@
         <v>133047</v>
       </c>
       <c r="B114" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C114" s="5" t="s">
         <v>265</v>
-      </c>
-      <c r="C114" s="5" t="s">
-        <v>266</v>
       </c>
       <c r="D114" s="5">
         <v>3</v>
@@ -10600,10 +10601,10 @@
         <v>133048</v>
       </c>
       <c r="B115" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C115" s="5" t="s">
         <v>267</v>
-      </c>
-      <c r="C115" s="5" t="s">
-        <v>268</v>
       </c>
       <c r="D115" s="5">
         <v>3</v>
@@ -10666,10 +10667,10 @@
         <v>133049</v>
       </c>
       <c r="B116" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C116" s="7" t="s">
         <v>269</v>
-      </c>
-      <c r="C116" s="7" t="s">
-        <v>270</v>
       </c>
       <c r="D116" s="5">
         <v>3</v>
@@ -10734,10 +10735,10 @@
         <v>133050</v>
       </c>
       <c r="B117" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C117" s="14" t="s">
         <v>271</v>
-      </c>
-      <c r="C117" s="14" t="s">
-        <v>272</v>
       </c>
       <c r="D117" s="5">
         <v>3</v>
@@ -10800,10 +10801,10 @@
         <v>133051</v>
       </c>
       <c r="B118" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C118" s="14" t="s">
         <v>273</v>
-      </c>
-      <c r="C118" s="14" t="s">
-        <v>274</v>
       </c>
       <c r="D118" s="5">
         <v>3</v>
@@ -10866,10 +10867,10 @@
         <v>133052</v>
       </c>
       <c r="B119" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C119" s="14" t="s">
         <v>275</v>
-      </c>
-      <c r="C119" s="14" t="s">
-        <v>276</v>
       </c>
       <c r="D119" s="5">
         <v>3</v>
@@ -10932,10 +10933,10 @@
         <v>133053</v>
       </c>
       <c r="B120" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C120" s="14" t="s">
         <v>277</v>
-      </c>
-      <c r="C120" s="14" t="s">
-        <v>278</v>
       </c>
       <c r="D120" s="5">
         <v>3</v>
@@ -10998,10 +10999,10 @@
         <v>133054</v>
       </c>
       <c r="B121" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="C121" s="15" t="s">
         <v>279</v>
-      </c>
-      <c r="C121" s="15" t="s">
-        <v>280</v>
       </c>
       <c r="D121" s="5">
         <v>3</v>
@@ -11064,10 +11065,10 @@
         <v>133055</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C122" s="16" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D122" s="5">
         <v>3</v>
@@ -11130,10 +11131,10 @@
         <v>133056</v>
       </c>
       <c r="B123" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C123" s="16" t="s">
         <v>282</v>
-      </c>
-      <c r="C123" s="16" t="s">
-        <v>283</v>
       </c>
       <c r="D123" s="5">
         <v>3</v>
@@ -11196,10 +11197,10 @@
         <v>133057</v>
       </c>
       <c r="B124" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C124" s="16" t="s">
         <v>284</v>
-      </c>
-      <c r="C124" s="16" t="s">
-        <v>285</v>
       </c>
       <c r="D124" s="5">
         <v>3</v>
@@ -11262,10 +11263,10 @@
         <v>133058</v>
       </c>
       <c r="B125" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C125" s="17" t="s">
         <v>286</v>
-      </c>
-      <c r="C125" s="17" t="s">
-        <v>287</v>
       </c>
       <c r="D125" s="5">
         <v>3</v>
@@ -11332,10 +11333,10 @@
         <v>133059</v>
       </c>
       <c r="B126" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C126" s="17" t="s">
         <v>288</v>
-      </c>
-      <c r="C126" s="17" t="s">
-        <v>289</v>
       </c>
       <c r="D126" s="5">
         <v>3</v>
@@ -11398,10 +11399,10 @@
         <v>133060</v>
       </c>
       <c r="B127" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C127" s="5" t="s">
         <v>290</v>
-      </c>
-      <c r="C127" s="5" t="s">
-        <v>291</v>
       </c>
       <c r="D127" s="5">
         <v>3</v>
@@ -11464,10 +11465,10 @@
         <v>133084</v>
       </c>
       <c r="B128" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C128" s="5" t="s">
         <v>292</v>
-      </c>
-      <c r="C128" s="5" t="s">
-        <v>293</v>
       </c>
       <c r="D128" s="5">
         <v>3</v>
@@ -11528,10 +11529,10 @@
         <v>133085</v>
       </c>
       <c r="B129" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="C129" s="9" t="s">
         <v>294</v>
-      </c>
-      <c r="C129" s="9" t="s">
-        <v>295</v>
       </c>
       <c r="D129" s="5">
         <v>3</v>
@@ -11594,10 +11595,10 @@
         <v>133086</v>
       </c>
       <c r="B130" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C130" s="9" t="s">
         <v>296</v>
-      </c>
-      <c r="C130" s="9" t="s">
-        <v>297</v>
       </c>
       <c r="D130" s="5">
         <v>3</v>
@@ -11660,10 +11661,10 @@
         <v>133087</v>
       </c>
       <c r="B131" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C131" s="9" t="s">
         <v>298</v>
-      </c>
-      <c r="C131" s="9" t="s">
-        <v>299</v>
       </c>
       <c r="D131" s="5">
         <v>3</v>
@@ -11726,10 +11727,10 @@
         <v>133088</v>
       </c>
       <c r="B132" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C132" s="9" t="s">
         <v>300</v>
-      </c>
-      <c r="C132" s="9" t="s">
-        <v>301</v>
       </c>
       <c r="D132" s="5">
         <v>3</v>
@@ -11792,10 +11793,10 @@
         <v>133089</v>
       </c>
       <c r="B133" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C133" s="9" t="s">
         <v>302</v>
-      </c>
-      <c r="C133" s="9" t="s">
-        <v>303</v>
       </c>
       <c r="D133" s="5">
         <v>3</v>
@@ -11858,10 +11859,10 @@
         <v>133090</v>
       </c>
       <c r="B134" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C134" s="9" t="s">
         <v>304</v>
-      </c>
-      <c r="C134" s="9" t="s">
-        <v>305</v>
       </c>
       <c r="D134" s="5">
         <v>3</v>
@@ -11924,10 +11925,10 @@
         <v>133091</v>
       </c>
       <c r="B135" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C135" s="9" t="s">
         <v>306</v>
-      </c>
-      <c r="C135" s="9" t="s">
-        <v>307</v>
       </c>
       <c r="D135" s="5">
         <v>3</v>
@@ -11990,10 +11991,10 @@
         <v>133092</v>
       </c>
       <c r="B136" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C136" s="9" t="s">
         <v>308</v>
-      </c>
-      <c r="C136" s="9" t="s">
-        <v>309</v>
       </c>
       <c r="D136" s="5">
         <v>3</v>
@@ -12056,10 +12057,10 @@
         <v>133093</v>
       </c>
       <c r="B137" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C137" s="9" t="s">
         <v>310</v>
-      </c>
-      <c r="C137" s="9" t="s">
-        <v>311</v>
       </c>
       <c r="D137" s="5">
         <v>3</v>
@@ -12122,10 +12123,10 @@
         <v>133094</v>
       </c>
       <c r="B138" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C138" s="5" t="s">
         <v>312</v>
-      </c>
-      <c r="C138" s="5" t="s">
-        <v>313</v>
       </c>
       <c r="D138" s="5">
         <v>3</v>
@@ -12188,10 +12189,10 @@
         <v>133095</v>
       </c>
       <c r="B139" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="C139" s="5" t="s">
         <v>314</v>
-      </c>
-      <c r="C139" s="5" t="s">
-        <v>315</v>
       </c>
       <c r="D139" s="5">
         <v>3</v>
@@ -12254,10 +12255,10 @@
         <v>133096</v>
       </c>
       <c r="B140" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C140" s="5" t="s">
         <v>316</v>
-      </c>
-      <c r="C140" s="5" t="s">
-        <v>317</v>
       </c>
       <c r="D140" s="5">
         <v>3</v>
@@ -12320,10 +12321,10 @@
         <v>133097</v>
       </c>
       <c r="B141" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C141" s="5" t="s">
         <v>318</v>
-      </c>
-      <c r="C141" s="5" t="s">
-        <v>319</v>
       </c>
       <c r="D141" s="5">
         <v>3</v>
@@ -12386,10 +12387,10 @@
         <v>133098</v>
       </c>
       <c r="B142" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="C142" s="5" t="s">
         <v>320</v>
-      </c>
-      <c r="C142" s="5" t="s">
-        <v>321</v>
       </c>
       <c r="D142" s="5">
         <v>3</v>
@@ -12452,10 +12453,10 @@
         <v>133099</v>
       </c>
       <c r="B143" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C143" s="5" t="s">
         <v>322</v>
-      </c>
-      <c r="C143" s="5" t="s">
-        <v>323</v>
       </c>
       <c r="D143" s="5">
         <v>3</v>
@@ -12518,10 +12519,10 @@
         <v>133100</v>
       </c>
       <c r="B144" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="C144" s="18" t="s">
         <v>324</v>
-      </c>
-      <c r="C144" s="18" t="s">
-        <v>325</v>
       </c>
       <c r="D144" s="18">
         <v>3</v>
@@ -12584,10 +12585,10 @@
         <v>133101</v>
       </c>
       <c r="B145" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="C145" s="18" t="s">
         <v>326</v>
-      </c>
-      <c r="C145" s="18" t="s">
-        <v>327</v>
       </c>
       <c r="D145" s="18">
         <v>3</v>
@@ -12650,10 +12651,10 @@
         <v>133102</v>
       </c>
       <c r="B146" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="C146" s="18" t="s">
         <v>328</v>
-      </c>
-      <c r="C146" s="18" t="s">
-        <v>329</v>
       </c>
       <c r="D146" s="18">
         <v>3</v>
@@ -12716,10 +12717,10 @@
         <v>133103</v>
       </c>
       <c r="B147" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="C147" s="18" t="s">
         <v>330</v>
-      </c>
-      <c r="C147" s="18" t="s">
-        <v>331</v>
       </c>
       <c r="D147" s="18">
         <v>3</v>
@@ -12782,10 +12783,10 @@
         <v>133104</v>
       </c>
       <c r="B148" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="C148" s="18" t="s">
         <v>332</v>
-      </c>
-      <c r="C148" s="18" t="s">
-        <v>333</v>
       </c>
       <c r="D148" s="18">
         <v>3</v>
@@ -12848,10 +12849,10 @@
         <v>133105</v>
       </c>
       <c r="B149" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="C149" s="18" t="s">
         <v>334</v>
-      </c>
-      <c r="C149" s="18" t="s">
-        <v>335</v>
       </c>
       <c r="D149" s="18">
         <v>3</v>
@@ -12914,10 +12915,10 @@
         <v>133106</v>
       </c>
       <c r="B150" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="C150" s="18" t="s">
         <v>336</v>
-      </c>
-      <c r="C150" s="18" t="s">
-        <v>337</v>
       </c>
       <c r="D150" s="18">
         <v>3</v>
@@ -12980,10 +12981,10 @@
         <v>133107</v>
       </c>
       <c r="B151" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="C151" s="20" t="s">
         <v>338</v>
-      </c>
-      <c r="C151" s="20" t="s">
-        <v>339</v>
       </c>
       <c r="D151" s="18">
         <v>3</v>
@@ -13046,10 +13047,10 @@
         <v>133108</v>
       </c>
       <c r="B152" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="C152" s="20" t="s">
         <v>340</v>
-      </c>
-      <c r="C152" s="20" t="s">
-        <v>341</v>
       </c>
       <c r="D152" s="18">
         <v>3</v>
@@ -13112,10 +13113,10 @@
         <v>133109</v>
       </c>
       <c r="B153" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="C153" s="20" t="s">
         <v>342</v>
-      </c>
-      <c r="C153" s="20" t="s">
-        <v>343</v>
       </c>
       <c r="D153" s="18">
         <v>3</v>
@@ -13178,10 +13179,10 @@
         <v>133110</v>
       </c>
       <c r="B154" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="C154" s="20" t="s">
         <v>344</v>
-      </c>
-      <c r="C154" s="20" t="s">
-        <v>345</v>
       </c>
       <c r="D154" s="18">
         <v>3</v>
@@ -13244,10 +13245,10 @@
         <v>133111</v>
       </c>
       <c r="B155" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="C155" s="20" t="s">
         <v>346</v>
-      </c>
-      <c r="C155" s="20" t="s">
-        <v>347</v>
       </c>
       <c r="D155" s="18">
         <v>3</v>
@@ -13310,10 +13311,10 @@
         <v>133112</v>
       </c>
       <c r="B156" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="C156" s="20" t="s">
         <v>348</v>
-      </c>
-      <c r="C156" s="20" t="s">
-        <v>349</v>
       </c>
       <c r="D156" s="18">
         <v>3</v>
@@ -13376,10 +13377,10 @@
         <v>133113</v>
       </c>
       <c r="B157" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="C157" s="18" t="s">
         <v>350</v>
-      </c>
-      <c r="C157" s="18" t="s">
-        <v>351</v>
       </c>
       <c r="D157" s="18">
         <v>3</v>
@@ -13442,10 +13443,10 @@
         <v>133114</v>
       </c>
       <c r="B158" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="C158" s="18" t="s">
         <v>352</v>
-      </c>
-      <c r="C158" s="18" t="s">
-        <v>353</v>
       </c>
       <c r="D158" s="18">
         <v>3</v>
@@ -13508,10 +13509,10 @@
         <v>133115</v>
       </c>
       <c r="B159" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="C159" s="18" t="s">
         <v>354</v>
-      </c>
-      <c r="C159" s="18" t="s">
-        <v>355</v>
       </c>
       <c r="D159" s="18">
         <v>3</v>
@@ -13574,10 +13575,10 @@
         <v>133116</v>
       </c>
       <c r="B160" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="C160" s="20" t="s">
         <v>356</v>
-      </c>
-      <c r="C160" s="20" t="s">
-        <v>357</v>
       </c>
       <c r="D160" s="18">
         <v>3</v>
@@ -13640,10 +13641,10 @@
         <v>133117</v>
       </c>
       <c r="B161" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="C161" s="18" t="s">
         <v>358</v>
-      </c>
-      <c r="C161" s="18" t="s">
-        <v>359</v>
       </c>
       <c r="D161" s="18">
         <v>3</v>
@@ -13706,10 +13707,10 @@
         <v>133118</v>
       </c>
       <c r="B162" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="C162" s="18" t="s">
         <v>360</v>
-      </c>
-      <c r="C162" s="18" t="s">
-        <v>361</v>
       </c>
       <c r="D162" s="18">
         <v>3</v>
@@ -13772,10 +13773,10 @@
         <v>133119</v>
       </c>
       <c r="B163" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="C163" s="18" t="s">
         <v>362</v>
-      </c>
-      <c r="C163" s="18" t="s">
-        <v>363</v>
       </c>
       <c r="D163" s="18">
         <v>3</v>
@@ -13838,10 +13839,10 @@
         <v>133120</v>
       </c>
       <c r="B164" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="C164" s="18" t="s">
         <v>364</v>
-      </c>
-      <c r="C164" s="18" t="s">
-        <v>365</v>
       </c>
       <c r="D164" s="18">
         <v>3</v>
@@ -13904,10 +13905,10 @@
         <v>133121</v>
       </c>
       <c r="B165" s="18" t="s">
+        <v>365</v>
+      </c>
+      <c r="C165" s="18" t="s">
         <v>366</v>
-      </c>
-      <c r="C165" s="18" t="s">
-        <v>367</v>
       </c>
       <c r="D165" s="18">
         <v>3</v>
@@ -13970,10 +13971,10 @@
         <v>133122</v>
       </c>
       <c r="B166" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="C166" s="18" t="s">
         <v>368</v>
-      </c>
-      <c r="C166" s="18" t="s">
-        <v>369</v>
       </c>
       <c r="D166" s="18">
         <v>3</v>
@@ -14036,10 +14037,10 @@
         <v>133123</v>
       </c>
       <c r="B167" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="C167" s="5" t="s">
         <v>370</v>
-      </c>
-      <c r="C167" s="5" t="s">
-        <v>371</v>
       </c>
       <c r="D167" s="5">
         <v>3</v>
@@ -14102,10 +14103,10 @@
         <v>133124</v>
       </c>
       <c r="B168" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="C168" s="5" t="s">
         <v>372</v>
-      </c>
-      <c r="C168" s="5" t="s">
-        <v>373</v>
       </c>
       <c r="D168" s="5">
         <v>3</v>
@@ -14168,10 +14169,10 @@
         <v>133125</v>
       </c>
       <c r="B169" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="C169" s="5" t="s">
         <v>374</v>
-      </c>
-      <c r="C169" s="5" t="s">
-        <v>375</v>
       </c>
       <c r="D169" s="5">
         <v>3</v>
@@ -14234,10 +14235,10 @@
         <v>133126</v>
       </c>
       <c r="B170" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="C170" s="5" t="s">
         <v>376</v>
-      </c>
-      <c r="C170" s="5" t="s">
-        <v>377</v>
       </c>
       <c r="D170" s="5">
         <v>3</v>
@@ -14300,10 +14301,10 @@
         <v>133127</v>
       </c>
       <c r="B171" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="C171" s="5" t="s">
         <v>378</v>
-      </c>
-      <c r="C171" s="5" t="s">
-        <v>379</v>
       </c>
       <c r="D171" s="5">
         <v>3</v>
@@ -14366,10 +14367,10 @@
         <v>133128</v>
       </c>
       <c r="B172" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="C172" s="5" t="s">
         <v>380</v>
-      </c>
-      <c r="C172" s="5" t="s">
-        <v>381</v>
       </c>
       <c r="D172" s="5">
         <v>3</v>
@@ -14432,10 +14433,10 @@
         <v>133129</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D173" s="5">
         <v>3</v>
@@ -14502,10 +14503,10 @@
         <v>133130</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D174" s="5">
         <v>3</v>
@@ -14568,10 +14569,10 @@
         <v>133131</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D175" s="5">
         <v>3</v>
@@ -14634,10 +14635,10 @@
         <v>133132</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D176" s="5">
         <v>3</v>
@@ -14700,10 +14701,10 @@
         <v>133133</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D177" s="5">
         <v>3</v>
@@ -14766,10 +14767,10 @@
         <v>133134</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D178" s="5">
         <v>3</v>
@@ -14832,10 +14833,10 @@
         <v>133135</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D179" s="5">
         <v>3</v>
@@ -14898,10 +14899,10 @@
         <v>133136</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C180" s="17" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D180" s="5">
         <v>3</v>
@@ -14968,10 +14969,10 @@
         <v>133137</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C181" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D181" s="5">
         <v>3</v>
@@ -15034,10 +15035,10 @@
         <v>133138</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D182" s="5">
         <v>3</v>
@@ -15100,10 +15101,10 @@
         <v>133139</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D183" s="5">
         <v>3</v>
@@ -15166,10 +15167,10 @@
         <v>133140</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D184" s="5">
         <v>3</v>
@@ -15232,10 +15233,10 @@
         <v>133141</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D185" s="5">
         <v>3</v>
@@ -15298,10 +15299,10 @@
         <v>133142</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D186" s="5">
         <v>3</v>
@@ -15364,10 +15365,10 @@
         <v>133143</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D187" s="5">
         <v>3</v>
@@ -15430,10 +15431,10 @@
         <v>133144</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D188" s="5">
         <v>3</v>
@@ -15496,10 +15497,10 @@
         <v>133145</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C189" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D189" s="5">
         <v>3</v>
@@ -15562,10 +15563,10 @@
         <v>133146</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D190" s="5">
         <v>3</v>
@@ -15628,10 +15629,10 @@
         <v>133147</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D191" s="5">
         <v>3</v>
@@ -15694,10 +15695,10 @@
         <v>133148</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D192" s="5">
         <v>3</v>
@@ -15760,10 +15761,10 @@
         <v>134001</v>
       </c>
       <c r="B193" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="C193" s="5" t="s">
         <v>528</v>
-      </c>
-      <c r="C193" s="5" t="s">
-        <v>529</v>
       </c>
       <c r="D193" s="5">
         <v>4</v>
@@ -15826,10 +15827,10 @@
         <v>134002</v>
       </c>
       <c r="B194" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="C194" s="5" t="s">
         <v>382</v>
-      </c>
-      <c r="C194" s="5" t="s">
-        <v>383</v>
       </c>
       <c r="D194" s="5">
         <v>4</v>
@@ -15892,10 +15893,10 @@
         <v>134003</v>
       </c>
       <c r="B195" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="C195" s="5" t="s">
         <v>384</v>
-      </c>
-      <c r="C195" s="5" t="s">
-        <v>385</v>
       </c>
       <c r="D195" s="5">
         <v>4</v>
@@ -15958,10 +15959,10 @@
         <v>134004</v>
       </c>
       <c r="B196" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C196" s="5" t="s">
         <v>386</v>
-      </c>
-      <c r="C196" s="5" t="s">
-        <v>387</v>
       </c>
       <c r="D196" s="5">
         <v>4</v>
@@ -16024,10 +16025,10 @@
         <v>134005</v>
       </c>
       <c r="B197" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="C197" s="5" t="s">
         <v>388</v>
-      </c>
-      <c r="C197" s="5" t="s">
-        <v>389</v>
       </c>
       <c r="D197" s="5">
         <v>4</v>
@@ -16090,10 +16091,10 @@
         <v>134006</v>
       </c>
       <c r="B198" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="C198" s="5" t="s">
         <v>390</v>
-      </c>
-      <c r="C198" s="5" t="s">
-        <v>391</v>
       </c>
       <c r="D198" s="5">
         <v>4</v>
@@ -16156,10 +16157,10 @@
         <v>134007</v>
       </c>
       <c r="B199" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="C199" s="5" t="s">
         <v>392</v>
-      </c>
-      <c r="C199" s="5" t="s">
-        <v>393</v>
       </c>
       <c r="D199" s="5">
         <v>4</v>
@@ -16222,10 +16223,10 @@
         <v>134008</v>
       </c>
       <c r="B200" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="C200" s="5" t="s">
         <v>394</v>
-      </c>
-      <c r="C200" s="5" t="s">
-        <v>395</v>
       </c>
       <c r="D200" s="5">
         <v>4</v>
@@ -16288,10 +16289,10 @@
         <v>134009</v>
       </c>
       <c r="B201" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="C201" s="5" t="s">
         <v>396</v>
-      </c>
-      <c r="C201" s="5" t="s">
-        <v>397</v>
       </c>
       <c r="D201" s="5">
         <v>4</v>
@@ -16354,10 +16355,10 @@
         <v>134010</v>
       </c>
       <c r="B202" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="C202" s="5" t="s">
         <v>398</v>
-      </c>
-      <c r="C202" s="5" t="s">
-        <v>399</v>
       </c>
       <c r="D202" s="5">
         <v>4</v>
@@ -16420,10 +16421,10 @@
         <v>135088</v>
       </c>
       <c r="B203" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="C203" s="5" t="s">
         <v>400</v>
-      </c>
-      <c r="C203" s="5" t="s">
-        <v>401</v>
       </c>
       <c r="D203" s="5">
         <v>5</v>
@@ -16484,10 +16485,10 @@
         <v>135089</v>
       </c>
       <c r="B204" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C204" s="5" t="s">
         <v>402</v>
-      </c>
-      <c r="C204" s="5" t="s">
-        <v>403</v>
       </c>
       <c r="D204" s="5">
         <v>5</v>
@@ -16548,10 +16549,10 @@
         <v>135090</v>
       </c>
       <c r="B205" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="C205" s="5" t="s">
         <v>404</v>
-      </c>
-      <c r="C205" s="5" t="s">
-        <v>405</v>
       </c>
       <c r="D205" s="5">
         <v>5</v>
@@ -16612,10 +16613,10 @@
         <v>135091</v>
       </c>
       <c r="B206" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="C206" s="5" t="s">
         <v>406</v>
-      </c>
-      <c r="C206" s="5" t="s">
-        <v>407</v>
       </c>
       <c r="D206" s="5">
         <v>5</v>
@@ -16676,10 +16677,10 @@
         <v>135092</v>
       </c>
       <c r="B207" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="C207" s="5" t="s">
         <v>408</v>
-      </c>
-      <c r="C207" s="5" t="s">
-        <v>409</v>
       </c>
       <c r="D207" s="5">
         <v>5</v>
@@ -16740,10 +16741,10 @@
         <v>135093</v>
       </c>
       <c r="B208" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="C208" s="5" t="s">
         <v>410</v>
-      </c>
-      <c r="C208" s="5" t="s">
-        <v>411</v>
       </c>
       <c r="D208" s="5">
         <v>5</v>
@@ -16804,10 +16805,10 @@
         <v>136001</v>
       </c>
       <c r="B209" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="C209" s="5" t="s">
         <v>412</v>
-      </c>
-      <c r="C209" s="5" t="s">
-        <v>413</v>
       </c>
       <c r="D209" s="5">
         <v>6</v>
@@ -16872,10 +16873,10 @@
         <v>136002</v>
       </c>
       <c r="B210" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="C210" s="5" t="s">
         <v>414</v>
-      </c>
-      <c r="C210" s="5" t="s">
-        <v>415</v>
       </c>
       <c r="D210" s="5">
         <v>6</v>
@@ -16940,10 +16941,10 @@
         <v>136003</v>
       </c>
       <c r="B211" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="C211" s="5" t="s">
         <v>416</v>
-      </c>
-      <c r="C211" s="5" t="s">
-        <v>417</v>
       </c>
       <c r="D211" s="5">
         <v>6</v>
@@ -17008,10 +17009,10 @@
         <v>136004</v>
       </c>
       <c r="B212" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="C212" s="5" t="s">
         <v>418</v>
-      </c>
-      <c r="C212" s="5" t="s">
-        <v>419</v>
       </c>
       <c r="D212" s="5">
         <v>6</v>
@@ -17076,10 +17077,10 @@
         <v>136005</v>
       </c>
       <c r="B213" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="C213" s="5" t="s">
         <v>420</v>
-      </c>
-      <c r="C213" s="5" t="s">
-        <v>421</v>
       </c>
       <c r="D213" s="5">
         <v>6</v>
@@ -17144,10 +17145,10 @@
         <v>136006</v>
       </c>
       <c r="B214" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="C214" s="5" t="s">
         <v>422</v>
-      </c>
-      <c r="C214" s="5" t="s">
-        <v>423</v>
       </c>
       <c r="D214" s="5">
         <v>6</v>
@@ -17212,10 +17213,10 @@
         <v>136007</v>
       </c>
       <c r="B215" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="C215" s="5" t="s">
         <v>424</v>
-      </c>
-      <c r="C215" s="5" t="s">
-        <v>425</v>
       </c>
       <c r="D215" s="5">
         <v>6</v>
@@ -17280,10 +17281,10 @@
         <v>136008</v>
       </c>
       <c r="B216" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C216" s="5" t="s">
         <v>426</v>
-      </c>
-      <c r="C216" s="5" t="s">
-        <v>427</v>
       </c>
       <c r="D216" s="5">
         <v>6</v>
@@ -17348,10 +17349,10 @@
         <v>136009</v>
       </c>
       <c r="B217" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="C217" s="5" t="s">
         <v>428</v>
-      </c>
-      <c r="C217" s="5" t="s">
-        <v>429</v>
       </c>
       <c r="D217" s="5">
         <v>6</v>
@@ -17416,10 +17417,10 @@
         <v>136010</v>
       </c>
       <c r="B218" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="C218" s="5" t="s">
         <v>430</v>
-      </c>
-      <c r="C218" s="5" t="s">
-        <v>431</v>
       </c>
       <c r="D218" s="5">
         <v>6</v>
@@ -17484,10 +17485,10 @@
         <v>136011</v>
       </c>
       <c r="B219" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="C219" s="5" t="s">
         <v>432</v>
-      </c>
-      <c r="C219" s="5" t="s">
-        <v>433</v>
       </c>
       <c r="D219" s="5">
         <v>6</v>
@@ -17552,10 +17553,10 @@
         <v>136012</v>
       </c>
       <c r="B220" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="C220" s="5" t="s">
         <v>434</v>
-      </c>
-      <c r="C220" s="5" t="s">
-        <v>435</v>
       </c>
       <c r="D220" s="5">
         <v>6</v>
@@ -17620,10 +17621,10 @@
         <v>136013</v>
       </c>
       <c r="B221" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="C221" s="5" t="s">
         <v>436</v>
-      </c>
-      <c r="C221" s="5" t="s">
-        <v>437</v>
       </c>
       <c r="D221" s="5">
         <v>6</v>
@@ -17688,10 +17689,10 @@
         <v>136014</v>
       </c>
       <c r="B222" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="C222" s="5" t="s">
         <v>438</v>
-      </c>
-      <c r="C222" s="5" t="s">
-        <v>439</v>
       </c>
       <c r="D222" s="5">
         <v>6</v>
@@ -17756,10 +17757,10 @@
         <v>136015</v>
       </c>
       <c r="B223" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="C223" s="5" t="s">
         <v>440</v>
-      </c>
-      <c r="C223" s="5" t="s">
-        <v>441</v>
       </c>
       <c r="D223" s="5">
         <v>6</v>
@@ -17824,10 +17825,10 @@
         <v>136016</v>
       </c>
       <c r="B224" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="C224" s="5" t="s">
         <v>442</v>
-      </c>
-      <c r="C224" s="5" t="s">
-        <v>443</v>
       </c>
       <c r="D224" s="5">
         <v>6</v>
@@ -17892,10 +17893,10 @@
         <v>136017</v>
       </c>
       <c r="B225" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="C225" s="5" t="s">
         <v>444</v>
-      </c>
-      <c r="C225" s="5" t="s">
-        <v>445</v>
       </c>
       <c r="D225" s="5">
         <v>6</v>
@@ -17960,10 +17961,10 @@
         <v>136018</v>
       </c>
       <c r="B226" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="C226" s="5" t="s">
         <v>446</v>
-      </c>
-      <c r="C226" s="5" t="s">
-        <v>447</v>
       </c>
       <c r="D226" s="5">
         <v>6</v>
@@ -18028,10 +18029,10 @@
         <v>136019</v>
       </c>
       <c r="B227" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="C227" s="5" t="s">
         <v>448</v>
-      </c>
-      <c r="C227" s="5" t="s">
-        <v>449</v>
       </c>
       <c r="D227" s="5">
         <v>6</v>
@@ -18096,10 +18097,10 @@
         <v>136020</v>
       </c>
       <c r="B228" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="C228" s="5" t="s">
         <v>450</v>
-      </c>
-      <c r="C228" s="5" t="s">
-        <v>451</v>
       </c>
       <c r="D228" s="5">
         <v>6</v>
@@ -18164,10 +18165,10 @@
         <v>136021</v>
       </c>
       <c r="B229" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="C229" s="5" t="s">
         <v>452</v>
-      </c>
-      <c r="C229" s="5" t="s">
-        <v>453</v>
       </c>
       <c r="D229" s="5">
         <v>6</v>
@@ -18232,10 +18233,10 @@
         <v>136022</v>
       </c>
       <c r="B230" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="C230" s="5" t="s">
         <v>454</v>
-      </c>
-      <c r="C230" s="5" t="s">
-        <v>455</v>
       </c>
       <c r="D230" s="5">
         <v>6</v>
@@ -18300,10 +18301,10 @@
         <v>136023</v>
       </c>
       <c r="B231" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C231" s="5" t="s">
         <v>456</v>
-      </c>
-      <c r="C231" s="5" t="s">
-        <v>457</v>
       </c>
       <c r="D231" s="5">
         <v>6</v>
@@ -18368,10 +18369,10 @@
         <v>136024</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C232" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D232" s="5">
         <v>6</v>
@@ -18434,10 +18435,10 @@
         <v>136025</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C233" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D233" s="5">
         <v>6</v>
@@ -18500,10 +18501,10 @@
         <v>136026</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C234" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D234" s="5">
         <v>6</v>
@@ -18566,10 +18567,10 @@
         <v>136027</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C235" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D235" s="5">
         <v>6</v>
@@ -18632,10 +18633,10 @@
         <v>136028</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C236" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D236" s="5">
         <v>6</v>
@@ -18698,10 +18699,10 @@
         <v>136029</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C237" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D237" s="5">
         <v>6</v>
@@ -18764,10 +18765,10 @@
         <v>136030</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C238" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D238" s="5">
         <v>6</v>
@@ -18830,10 +18831,10 @@
         <v>136031</v>
       </c>
       <c r="B239" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C239" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D239" s="5">
         <v>6</v>
@@ -18897,7 +18898,7 @@
       </c>
       <c r="B240" s="5"/>
       <c r="C240" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D240" s="5">
         <v>7</v>
@@ -18955,7 +18956,7 @@
       </c>
       <c r="B241" s="5"/>
       <c r="C241" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D241" s="5">
         <v>7</v>
@@ -19013,7 +19014,7 @@
       </c>
       <c r="B242" s="5"/>
       <c r="C242" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D242" s="5">
         <v>7</v>
@@ -19071,7 +19072,7 @@
       </c>
       <c r="B243" s="5"/>
       <c r="C243" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D243" s="5">
         <v>7</v>
@@ -19129,7 +19130,7 @@
       </c>
       <c r="B244" s="5"/>
       <c r="C244" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D244" s="5">
         <v>7</v>
@@ -19187,7 +19188,7 @@
       </c>
       <c r="B245" s="5"/>
       <c r="C245" s="5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D245" s="5">
         <v>7</v>
@@ -19245,7 +19246,7 @@
       </c>
       <c r="B246" s="5"/>
       <c r="C246" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D246" s="5">
         <v>7</v>

</xml_diff>